<commit_message>
# deletePet using excel
</commit_message>
<xml_diff>
--- a/src/test/java/petStore/testData/addNewPetData.xlsx
+++ b/src/test/java/petStore/testData/addNewPetData.xlsx
@@ -53,21 +53,6 @@
     <t>addNewPetTest_005</t>
   </si>
   <si>
-    <t>Larry</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Ron</t>
-  </si>
-  <si>
-    <t>Snape</t>
-  </si>
-  <si>
-    <t>Dumbledor</t>
-  </si>
-  <si>
     <t>sold</t>
   </si>
   <si>
@@ -78,6 +63,21 @@
   </si>
   <si>
     <t>wrong</t>
+  </si>
+  <si>
+    <t>Merry</t>
+  </si>
+  <si>
+    <t>Pippin</t>
+  </si>
+  <si>
+    <t>Aragorn</t>
+  </si>
+  <si>
+    <t>Gimli</t>
+  </si>
+  <si>
+    <t>Legolas</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,10 +448,10 @@
         <v>100001</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -462,10 +462,10 @@
         <v>100002</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -476,10 +476,10 @@
         <v>100003</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,10 +490,10 @@
         <v>100004</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,10 +504,10 @@
         <v>100005</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>